<commit_message>
made updates to Vermont
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gpain/Documents/Work_Dashboards/Alaska/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gpain/Documents/Work_Dashboards/Vermont/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23C295C-9E42-B24B-B17C-05856C82CD9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17F5FB0-2CB7-3244-ABEB-8B8D8BE4D5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{949A1E6F-A50E-0D47-B806-7BF7EBA35A5B}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{949A1E6F-A50E-0D47-B806-7BF7EBA35A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="423">
   <si>
     <t>table_name</t>
   </si>
@@ -1271,12 +1271,114 @@
   <si>
     <t>prgm_url</t>
   </si>
+  <si>
+    <t>Internal training provided for staff and/or board</t>
+  </si>
+  <si>
+    <t>External training provided by organization to community</t>
+  </si>
+  <si>
+    <t>Program or curriculum revision</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In planning stages</t>
+  </si>
+  <si>
+    <t>New partnerships</t>
+  </si>
+  <si>
+    <t>Staff or board diversification</t>
+  </si>
+  <si>
+    <t>More inclusive marketing</t>
+  </si>
+  <si>
+    <t>Internal Training</t>
+  </si>
+  <si>
+    <t>External Training</t>
+  </si>
+  <si>
+    <t>Program Revision</t>
+  </si>
+  <si>
+    <t>In Planning Stages</t>
+  </si>
+  <si>
+    <t>New Partnerships</t>
+  </si>
+  <si>
+    <t>Staff or Board Diversification</t>
+  </si>
+  <si>
+    <t>More Inclusive Marketing</t>
+  </si>
+  <si>
+    <t>Classroom volunteers/presenters</t>
+  </si>
+  <si>
+    <t>Curriculum &amp; instructional materials</t>
+  </si>
+  <si>
+    <t>Field trips</t>
+  </si>
+  <si>
+    <t>Materials &amp; supplies</t>
+  </si>
+  <si>
+    <t>Events/Symposiums</t>
+  </si>
+  <si>
+    <t>Professional development/consulting for administrators</t>
+  </si>
+  <si>
+    <t>Professional development/consulting for teachers</t>
+  </si>
+  <si>
+    <t>Supporting networks (online/in-person)</t>
+  </si>
+  <si>
+    <t>Materials &amp; Supplies</t>
+  </si>
+  <si>
+    <t>Professional Development for Admin</t>
+  </si>
+  <si>
+    <t>Professional Development for Teachers</t>
+  </si>
+  <si>
+    <t>Supporting Networks (online/in-person)</t>
+  </si>
+  <si>
+    <t>Mobility/wheelchair accommodations</t>
+  </si>
+  <si>
+    <t>Special education accommodations</t>
+  </si>
+  <si>
+    <t>Deaf/hearing-impaired accommodations</t>
+  </si>
+  <si>
+    <t>Blind/sight-impaired accommodations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobility </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Special education </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaf/hearing-impaired </t>
+  </si>
+  <si>
+    <t>Blind/sight-impaired</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1349,6 +1451,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF112337"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1403,7 +1511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1446,6 +1554,11 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2502,8 +2615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09851FDF-4334-4E44-81EF-4155DEF57BA3}">
   <dimension ref="A1:K122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="B95" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E119" sqref="E119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3754,7 +3867,7 @@
         <v>13</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H21" s="2">
         <v>0</v>
@@ -3764,7 +3877,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -3822,13 +3935,13 @@
         <v>14</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H23" s="2">
         <v>0</v>
       </c>
       <c r="J23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>13</v>
@@ -5620,7 +5733,7 @@
         <v>0</v>
       </c>
       <c r="J79" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K79" s="2" t="s">
         <v>13</v>
@@ -5652,7 +5765,7 @@
         <v>0</v>
       </c>
       <c r="J80" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K80" s="2" t="s">
         <v>13</v>
@@ -5678,7 +5791,7 @@
         <v>13</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H81" s="2">
         <v>0</v>
@@ -5745,13 +5858,16 @@
         <v>14</v>
       </c>
       <c r="H83" s="2">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="I83" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="J83" s="2">
         <v>0</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5934,16 +6050,16 @@
         <v>13</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H89" s="2">
         <v>0</v>
       </c>
       <c r="J89" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="90" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6504,10 +6620,10 @@
         <v>37</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G107" s="2" t="s">
         <v>14</v>
@@ -6536,10 +6652,10 @@
         <v>38</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G108" s="2" t="s">
         <v>14</v>
@@ -6568,10 +6684,10 @@
         <v>39</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G109" s="2" t="s">
         <v>14</v>
@@ -6600,10 +6716,10 @@
         <v>40</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G110" s="2" t="s">
         <v>14</v>
@@ -6632,10 +6748,10 @@
         <v>41</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G111" s="2" t="s">
         <v>14</v>
@@ -6664,10 +6780,10 @@
         <v>42</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G112" s="2" t="s">
         <v>14</v>
@@ -6696,10 +6812,10 @@
         <v>43</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G113" s="2" t="s">
         <v>14</v>
@@ -6728,10 +6844,10 @@
         <v>44</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G114" s="2" t="s">
         <v>14</v>
@@ -6760,10 +6876,10 @@
         <v>45</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G115" s="2" t="s">
         <v>14</v>
@@ -6792,10 +6908,10 @@
         <v>46</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G116" s="2" t="s">
         <v>14</v>
@@ -6824,10 +6940,10 @@
         <v>47</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G117" s="2" t="s">
         <v>14</v>
@@ -6865,17 +6981,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D1373AD-CAFE-FC46-B12F-4E16ECB9F9F7}">
-  <dimension ref="A1:N94"/>
+  <dimension ref="A1:N115"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" customWidth="1"/>
-    <col min="4" max="4" width="35.1640625" customWidth="1"/>
+    <col min="3" max="3" width="43.1640625" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="19.5" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
@@ -8241,16 +8357,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>39</v>
+        <v>212</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>13</v>
+        <v>389</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>13</v>
+        <v>396</v>
       </c>
       <c r="E47" s="2">
         <v>1</v>
@@ -8258,230 +8374,226 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>39</v>
+        <v>212</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>14</v>
+        <v>390</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>14</v>
+        <v>397</v>
       </c>
       <c r="E48" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>272</v>
+        <v>212</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>132</v>
+        <v>391</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>132</v>
+        <v>398</v>
       </c>
       <c r="E49" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>272</v>
+        <v>212</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>133</v>
+        <v>392</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>133</v>
+        <v>399</v>
       </c>
       <c r="E50" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>272</v>
+        <v>212</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>134</v>
+        <v>393</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>134</v>
+        <v>400</v>
       </c>
       <c r="E51" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>272</v>
+        <v>212</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>135</v>
+        <v>394</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>135</v>
+        <v>401</v>
       </c>
       <c r="E52" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>272</v>
+        <v>212</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>136</v>
+        <v>395</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>136</v>
+        <v>402</v>
       </c>
       <c r="E53" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B54" s="14" t="s">
-        <v>264</v>
+      <c r="B54" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>137</v>
+        <v>13</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>137</v>
+        <v>13</v>
       </c>
       <c r="E54" s="2">
         <v>1</v>
       </c>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B55" s="14" t="s">
-        <v>264</v>
+      <c r="B55" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>138</v>
+        <v>14</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>138</v>
+        <v>14</v>
       </c>
       <c r="E55" s="2">
         <v>2</v>
       </c>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B56" s="14" t="s">
-        <v>264</v>
+      <c r="B56" s="2" t="s">
+        <v>272</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E56" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E57" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E58" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B57" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E57" s="2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E59" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B58" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E58" s="2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E60" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B59" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E59" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B60" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E60" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>30</v>
       </c>
@@ -8489,16 +8601,18 @@
         <v>264</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E61" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>30</v>
       </c>
@@ -8506,25 +8620,18 @@
         <v>264</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="E62" s="2">
-        <v>9</v>
-      </c>
-      <c r="F62" s="16"/>
+        <v>2</v>
+      </c>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
-      <c r="J62" s="2"/>
-      <c r="K62" s="2"/>
-      <c r="L62" s="2"/>
-      <c r="M62" s="2"/>
-      <c r="N62" s="2"/>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>30</v>
       </c>
@@ -8532,16 +8639,16 @@
         <v>264</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="E63" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>30</v>
       </c>
@@ -8549,16 +8656,16 @@
         <v>264</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="E64" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>30</v>
       </c>
@@ -8566,16 +8673,16 @@
         <v>264</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E65" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>30</v>
       </c>
@@ -8583,16 +8690,16 @@
         <v>264</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="E66" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>30</v>
       </c>
@@ -8600,152 +8707,161 @@
         <v>264</v>
       </c>
       <c r="C67" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E67" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E68" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E69" s="2">
+        <v>9</v>
+      </c>
+      <c r="F69" s="16"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+      <c r="M69" s="2"/>
+      <c r="N69" s="2"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E70" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E71" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E72" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E73" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D74" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E67" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B68" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E68" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B69" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C69" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="D69" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="E69" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B70" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C70" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="D70" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="E70" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B71" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C71" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="D71" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="E71" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B72" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C72" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="D72" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="E72" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B73" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C73" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="D73" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="E73" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B74" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C74" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="D74" s="17" t="s">
-        <v>160</v>
-      </c>
       <c r="E74" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B75" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="C75" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="D75" s="17" t="s">
-        <v>162</v>
+      <c r="C75" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E75" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>30</v>
       </c>
@@ -8753,16 +8869,16 @@
         <v>270</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D76" s="17" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="E76" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>30</v>
       </c>
@@ -8770,16 +8886,16 @@
         <v>270</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="D77" s="17" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="E77" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>30</v>
       </c>
@@ -8787,16 +8903,16 @@
         <v>270</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="D78" s="17" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="E78" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>30</v>
       </c>
@@ -8804,16 +8920,16 @@
         <v>270</v>
       </c>
       <c r="C79" s="17" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="D79" s="17" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="E79" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>30</v>
       </c>
@@ -8821,13 +8937,13 @@
         <v>270</v>
       </c>
       <c r="C80" s="17" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="D80" s="17" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="E80" s="2">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -8838,13 +8954,13 @@
         <v>270</v>
       </c>
       <c r="C81" s="17" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="D81" s="17" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="E81" s="2">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -8854,14 +8970,14 @@
       <c r="B82" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="C82" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>175</v>
+      <c r="C82" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="D82" s="17" t="s">
+        <v>162</v>
       </c>
       <c r="E82" s="2">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -8871,14 +8987,14 @@
       <c r="B83" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="C83" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>176</v>
+      <c r="C83" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="D83" s="17" t="s">
+        <v>164</v>
       </c>
       <c r="E83" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -8888,14 +9004,14 @@
       <c r="B84" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="C84" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>177</v>
+      <c r="C84" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D84" s="17" t="s">
+        <v>166</v>
       </c>
       <c r="E84" s="2">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -8905,14 +9021,14 @@
       <c r="B85" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="C85" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>179</v>
+      <c r="C85" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="D85" s="17" t="s">
+        <v>168</v>
       </c>
       <c r="E85" s="2">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -8920,46 +9036,50 @@
         <v>30</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="C86" t="s">
-        <v>180</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E86" s="2"/>
+        <v>270</v>
+      </c>
+      <c r="C86" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="D86" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="E86" s="2">
+        <v>12</v>
+      </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B87" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E87" s="2"/>
+        <v>270</v>
+      </c>
+      <c r="C87" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D87" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="E87" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B88" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>183</v>
+        <v>270</v>
+      </c>
+      <c r="C88" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D88" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="E88" s="2">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -8967,16 +9087,16 @@
         <v>30</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="E89" s="2">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -8984,16 +9104,16 @@
         <v>30</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="E90" s="2">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -9001,16 +9121,16 @@
         <v>30</v>
       </c>
       <c r="B91" s="14" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="E91" s="2">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -9018,16 +9138,16 @@
         <v>30</v>
       </c>
       <c r="B92" s="14" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E92" s="2">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -9035,16 +9155,16 @@
         <v>30</v>
       </c>
       <c r="B93" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>188</v>
+        <v>279</v>
+      </c>
+      <c r="C93" t="s">
+        <v>180</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="E93" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -9052,16 +9172,373 @@
         <v>30</v>
       </c>
       <c r="B94" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E94" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B95" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E95" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B96" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C96" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E96" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B97" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E97" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B98" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E98" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B99" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E99" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B100" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E100" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B101" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C101" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D94" s="2" t="s">
+      <c r="D101" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E94" s="2">
+      <c r="E101" s="2">
         <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B102" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="E102" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B103" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="C103" s="20" t="s">
+        <v>404</v>
+      </c>
+      <c r="D103" s="20" t="s">
+        <v>404</v>
+      </c>
+      <c r="E103" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B104" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E104" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B105" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="E105" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B106" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="E106" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B107" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="E107" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B108" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="E108" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B109" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E109" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B110" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="E110" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B111" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="E111" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B112" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="E112" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B113" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C113" s="22" t="s">
+        <v>417</v>
+      </c>
+      <c r="D113" s="22" t="s">
+        <v>421</v>
+      </c>
+      <c r="E113" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B114" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C114" s="22" t="s">
+        <v>418</v>
+      </c>
+      <c r="D114" s="22" t="s">
+        <v>422</v>
+      </c>
+      <c r="E114" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B115" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E115" s="2">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>